<commit_message>
Validate becon service implemented.
</commit_message>
<xml_diff>
--- a/booking-engine-poi/src/main/resources/poidata/becon-data.xlsx
+++ b/booking-engine-poi/src/main/resources/poidata/becon-data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="22">
   <si>
     <t>uuid</t>
   </si>
@@ -73,6 +73,15 @@
   </si>
   <si>
     <t>St.Loius Airport shuttle 10</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>123</t>
   </si>
 </sst>
 </file>
@@ -415,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -449,7 +458,7 @@
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F3" s="1"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -472,7 +481,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -495,7 +504,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -518,7 +527,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -538,6 +547,98 @@
         <v>17</v>
       </c>
       <c r="G7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>